<commit_message>
reorganized plots, added spreadsheet
</commit_message>
<xml_diff>
--- a/Input_Data/Medicaid_managedcare_enrollment_report/external/mandate_tracker.xlsx
+++ b/Input_Data/Medicaid_managedcare_enrollment_report/external/mandate_tracker.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15060" windowHeight="5475"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14580" windowHeight="5475" tabRatio="663"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="81">
   <si>
     <t>State</t>
   </si>
@@ -182,38 +182,98 @@
     <t>Wyoming</t>
   </si>
   <si>
-    <t>Switched to no MMC</t>
-  </si>
-  <si>
-    <t>2016?</t>
-  </si>
-  <si>
-    <t>2013?</t>
-  </si>
-  <si>
     <t>No MMC</t>
   </si>
   <si>
-    <t>Already Mandated to 100% Pre 2001</t>
-  </si>
-  <si>
     <t>No Comprehensive MCO Until 2021</t>
   </si>
   <si>
-    <t>Huge Jump in Comprehensive MCO in One Year</t>
-  </si>
-  <si>
-    <t>Gradual Increase in Comprehensive MCO</t>
-  </si>
-  <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>Already Mandated to 100% Pre 2001 or Turned Off Treatment</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>https://medicaid.ms.gov/wp-content/uploads/2018/06/Managed-Care-Quality-Strat-and-Appendices-Initial-Draft-6.21.18.pdf</t>
+  </si>
+  <si>
+    <t>https://www.medicaid.gov/Medicaid/downloads/florida-mcp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.medicaid.gov/Medicaid/downloads/new-hampshire-mcp.pdf</t>
+  </si>
+  <si>
+    <t>https://hfs.illinois.gov/content/dam/soi/en/web/hfs/sitecollectiondocuments/il20212024comprehensivemedicalprogramsqualitystrategyd1.pdf</t>
+  </si>
+  <si>
+    <t>https://hhs.iowa.gov/media/12725/download?inline#:~:text=►On%20April%201%2C%202016,Care%20Organization%20(MCO)%20model.</t>
+  </si>
+  <si>
+    <t>https://www.medicaid.gov/Medicaid/downloads/kentucky-mcp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.medicaid.gov/Medicaid/downloads/louisiana-mcp.pdf</t>
+  </si>
+  <si>
+    <t>Year Expanded Post DH Mandate Data</t>
+  </si>
+  <si>
+    <t>Curve Type</t>
+  </si>
+  <si>
+    <t>big jump</t>
+  </si>
+  <si>
+    <t>gradual increase</t>
+  </si>
+  <si>
+    <t>https://mydss.mo.gov/mhd/hot-tips/managed-care-goes-statewide-may-1-2017#:~:text=Managed%20Care%20Goes%20Statewide%20on,2017%20%7C%20mydss.mo.gov</t>
+  </si>
+  <si>
+    <t>https://www.khi.org/wp-content/uploads/2024/01/Kansas-Medicaid-A-Primer-2024.pdf</t>
+  </si>
+  <si>
+    <t>https://www.medicaid.gov/Medicaid/downloads/ohio-mcp.pdf</t>
+  </si>
+  <si>
+    <t>https://www.medicaid.gov/Medicaid/downloads/south-carolina-mcp.pdf?utm_source=chatgpt.com</t>
+  </si>
+  <si>
+    <t>https://www.medicaid.gov/Medicaid/downloads/texas-mcp.pdf?utm_source=chatgpt.com</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Medicaid blind and disabled transitioned to risk based MCO in 2012</t>
+  </si>
+  <si>
+    <t>PCCM phased out of rural areas in favor of expanding STAR and STAR+PLUS programs statewide 2005-2011</t>
+  </si>
+  <si>
+    <t>Might need to FOIA or call</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>https://dhhs.ne.gov/Documents/NE%20Quality%20Strategy.pdf#:~:text=health%20and%20one%20for%20mental%20health%20and,Managed%20Care%20Organizations%20(MCOs)%20to%20deliver%20Medicaid</t>
+  </si>
+  <si>
+    <t>https://www.medicaid.gov/Medicaid/downloads/wisconsin-mcp.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,13 +289,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -247,14 +321,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -533,321 +616,814 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" customWidth="1"/>
-    <col min="4" max="4" width="44.28515625" customWidth="1"/>
-    <col min="5" max="5" width="38.140625" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="56.28515625" customWidth="1"/>
+    <col min="3" max="3" width="37" customWidth="1"/>
+    <col min="4" max="4" width="48.28515625" customWidth="1"/>
+    <col min="5" max="6" width="37" customWidth="1"/>
+    <col min="7" max="7" width="53.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11">
+        <v>2014</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12">
+        <v>2006</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15">
         <v>2018</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17">
+        <v>2016</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18">
+        <v>2013</v>
+      </c>
+      <c r="E18" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19">
+        <v>2012</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="2"/>
+      <c r="G19" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20">
         <v>2012</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26">
+        <v>2015</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="2"/>
+      <c r="G26" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" t="s">
+        <v>54</v>
+      </c>
+      <c r="D27">
+        <v>2017</v>
+      </c>
+      <c r="E27" t="s">
+        <v>68</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" t="s">
+        <v>78</v>
+      </c>
+      <c r="F28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29">
+        <v>2017</v>
+      </c>
+      <c r="E29" t="s">
+        <v>68</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31">
+        <v>2014</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37">
+        <v>2005</v>
+      </c>
+      <c r="E37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="C38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" t="s">
+        <v>54</v>
+      </c>
+      <c r="D42">
+        <v>2013</v>
+      </c>
+      <c r="E42" t="s">
+        <v>68</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45">
+        <v>2012</v>
+      </c>
+      <c r="E45" t="s">
+        <v>68</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" t="s">
+        <v>54</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" t="s">
+        <v>54</v>
+      </c>
+      <c r="F50" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51" t="s">
+        <v>54</v>
+      </c>
+      <c r="E51" t="s">
+        <v>68</v>
+      </c>
+      <c r="F51" t="s">
+        <v>77</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
+      <c r="B52" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" t="s">
+        <v>54</v>
+      </c>
+      <c r="D52" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G17" r:id="rId1" location=":~:text=►On%20April%201%2C%202016,Care%20Organization%20(MCO)%20model."/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
extended mandate data. No CA, CO, NY, and PA yet
</commit_message>
<xml_diff>
--- a/Input_Data/Medicaid_managedcare_enrollment_report/external/mandate_tracker.xlsx
+++ b/Input_Data/Medicaid_managedcare_enrollment_report/external/mandate_tracker.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="94">
   <si>
     <t>State</t>
   </si>
@@ -303,6 +303,12 @@
   </si>
   <si>
     <t>https://www.medicaid.gov/Medicaid/downloads/north-dakota-mcp.pdf?utm_source=chatgpt.com</t>
+  </si>
+  <si>
+    <t>https://www.medicaid.gov/Medicaid/downloads/minnesota-mcp.pdf</t>
+  </si>
+  <si>
+    <t>Not an official statewide mandate but by 2011, 2/3 of the Medicaid population was enrolled in an MCO plan (best thing I can find online and after making calls)</t>
   </si>
 </sst>
 </file>
@@ -654,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="C28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,7 +1119,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1123,11 +1129,17 @@
       <c r="C25" t="s">
         <v>54</v>
       </c>
+      <c r="D25">
+        <v>2011</v>
+      </c>
       <c r="E25" t="s">
         <v>80</v>
       </c>
-      <c r="F25" t="s">
-        <v>90</v>
+      <c r="F25" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1332,7 +1344,7 @@
       <c r="E36" t="s">
         <v>80</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="G36" s="4" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1639,8 +1651,9 @@
   <autoFilter ref="D1:D52"/>
   <hyperlinks>
     <hyperlink ref="G17" r:id="rId1" location=":~:text=►On%20April%201%2C%202016,Care%20Organization%20(MCO)%20model."/>
+    <hyperlink ref="G36" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added comments to did code
</commit_message>
<xml_diff>
--- a/Input_Data/Medicaid_managedcare_enrollment_report/external/mandate_tracker.xlsx
+++ b/Input_Data/Medicaid_managedcare_enrollment_report/external/mandate_tracker.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14580" windowHeight="5475" tabRatio="663"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9555" windowHeight="5085" tabRatio="663"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="95">
   <si>
     <t>State</t>
   </si>
@@ -293,12 +293,6 @@
     <t>https://pmc.ncbi.nlm.nih.gov/articles/PMC11198924/#:~:text=In%202021%2C%20North%20Carolina%20switched,the%20experience%20of%20Medicaid%20enrollees.</t>
   </si>
   <si>
-    <t>July 2011, more than half of West Virginia’s Medicaid beneficiaries were enrolled in one of three managed care</t>
-  </si>
-  <si>
-    <t>programs.</t>
-  </si>
-  <si>
     <t>Might need to call</t>
   </si>
   <si>
@@ -309,6 +303,15 @@
   </si>
   <si>
     <t>Not an official statewide mandate but by 2011, 2/3 of the Medicaid population was enrolled in an MCO plan (best thing I can find online and after making calls)</t>
+  </si>
+  <si>
+    <t>https://www.medicaid.gov/Medicaid/downloads/georgia-mcp.pdf</t>
+  </si>
+  <si>
+    <t>July 2011, more than half of West Virginia’s Medicaid beneficiaries were enrolled in one of three managed care programs</t>
+  </si>
+  <si>
+    <t>2017 potential treatment year</t>
   </si>
 </sst>
 </file>
@@ -660,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,7 +795,7 @@
         <v>54</v>
       </c>
       <c r="F6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -809,7 +812,7 @@
         <v>80</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -863,7 +866,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -880,7 +883,7 @@
         <v>78</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -901,6 +904,9 @@
         <v>78</v>
       </c>
       <c r="F12" s="2"/>
+      <c r="G12" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -933,7 +939,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -950,7 +956,7 @@
         <v>78</v>
       </c>
       <c r="F15" s="2"/>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="4" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1029,7 +1035,7 @@
         <v>78</v>
       </c>
       <c r="F19" s="2"/>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="4" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1136,10 +1142,10 @@
         <v>80</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1159,7 +1165,7 @@
         <v>78</v>
       </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="4" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1213,11 +1219,14 @@
       <c r="C29" t="s">
         <v>54</v>
       </c>
-      <c r="D29">
-        <v>2017</v>
+      <c r="D29" t="s">
+        <v>72</v>
       </c>
       <c r="E29" t="s">
         <v>80</v>
+      </c>
+      <c r="F29" t="s">
+        <v>94</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>73</v>
@@ -1233,6 +1242,9 @@
       <c r="C30" t="s">
         <v>54</v>
       </c>
+      <c r="D30" t="s">
+        <v>72</v>
+      </c>
       <c r="E30" t="s">
         <v>80</v>
       </c>
@@ -1301,11 +1313,14 @@
       <c r="C34" t="s">
         <v>54</v>
       </c>
+      <c r="D34" t="s">
+        <v>72</v>
+      </c>
       <c r="E34" t="s">
         <v>80</v>
       </c>
       <c r="F34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1324,7 +1339,7 @@
       <c r="E35" t="s">
         <v>78</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="G35" s="4" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1345,7 +1360,7 @@
         <v>80</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1364,7 +1379,7 @@
       <c r="E37" t="s">
         <v>80</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G37" s="4" t="s">
         <v>67</v>
       </c>
     </row>
@@ -1443,13 +1458,13 @@
       <c r="C42" t="s">
         <v>54</v>
       </c>
-      <c r="D42">
-        <v>2013</v>
+      <c r="D42" t="s">
+        <v>72</v>
       </c>
       <c r="E42" t="s">
         <v>80</v>
       </c>
-      <c r="G42" s="3" t="s">
+      <c r="G42" s="4" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1506,7 +1521,7 @@
       <c r="F45" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="G45" s="3" t="s">
+      <c r="G45" s="4" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1520,13 +1535,13 @@
       <c r="C46" t="s">
         <v>54</v>
       </c>
-      <c r="D46">
-        <v>2011</v>
+      <c r="D46" t="s">
+        <v>72</v>
       </c>
       <c r="E46" t="s">
         <v>78</v>
       </c>
-      <c r="G46" s="3" t="s">
+      <c r="G46" s="4" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1557,6 +1572,9 @@
       <c r="C48" t="s">
         <v>54</v>
       </c>
+      <c r="D48" t="s">
+        <v>72</v>
+      </c>
       <c r="E48" t="s">
         <v>80</v>
       </c>
@@ -1580,11 +1598,11 @@
       <c r="F49" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G49" s="3" t="s">
+      <c r="G49" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1594,14 +1612,14 @@
       <c r="C50" t="s">
         <v>54</v>
       </c>
-      <c r="D50">
-        <v>2011</v>
+      <c r="D50" t="s">
+        <v>72</v>
       </c>
       <c r="E50" t="s">
         <v>80</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1614,15 +1632,13 @@
       <c r="C51" t="s">
         <v>54</v>
       </c>
-      <c r="D51">
-        <v>2018</v>
+      <c r="D51" t="s">
+        <v>72</v>
       </c>
       <c r="E51" t="s">
         <v>80</v>
       </c>
-      <c r="F51" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="F51" s="3"/>
       <c r="G51" s="3" t="s">
         <v>85</v>
       </c>
@@ -1652,8 +1668,18 @@
   <hyperlinks>
     <hyperlink ref="G17" r:id="rId1" location=":~:text=►On%20April%201%2C%202016,Care%20Organization%20(MCO)%20model."/>
     <hyperlink ref="G36" r:id="rId2"/>
+    <hyperlink ref="G11" r:id="rId3"/>
+    <hyperlink ref="G15" r:id="rId4"/>
+    <hyperlink ref="G19" r:id="rId5"/>
+    <hyperlink ref="G26" r:id="rId6"/>
+    <hyperlink ref="G37" r:id="rId7"/>
+    <hyperlink ref="G42" r:id="rId8"/>
+    <hyperlink ref="G45" r:id="rId9"/>
+    <hyperlink ref="G46" r:id="rId10" location=":~:text=In%202011%2C%20Senate%20Bill%20180%2C%20Medicaid%20Reform%2C,delivery%20model%20with%20one%20or%20more%20risk%2Dbased"/>
+    <hyperlink ref="G49" r:id="rId11"/>
+    <hyperlink ref="G35" r:id="rId12" location=":~:text=In%202021%2C%20North%20Carolina%20switched,the%20experience%20of%20Medicaid%20enrollees."/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>